<commit_message>
update controllers, seeded questions
</commit_message>
<xml_diff>
--- a/documentation/CSAT Feedback Structure for DB.xlsx
+++ b/documentation/CSAT Feedback Structure for DB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Drive\WEBSITE_PROJECTS\_REPOS\_ASP.NET\CustomerFeedback\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C2284D60-5E71-4C83-85DA-DDDB5F191F36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9ED963E-24BF-45C5-8B30-DA85D05AF1F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1410" yWindow="1410" windowWidth="14010" windowHeight="8565" firstSheet="1" activeTab="2" xr2:uid="{65A720A9-0869-47F5-982B-4C93D77E8D45}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" firstSheet="1" activeTab="1" xr2:uid="{65A720A9-0869-47F5-982B-4C93D77E8D45}"/>
   </bookViews>
   <sheets>
     <sheet name="Survey Tracking and Scheduling" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,6 @@
     <sheet name="Sheet1" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1519,8 +1518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8E587CC-8B7F-4D6B-A6D2-CE9BBF242BFF}">
   <dimension ref="A1:E125"/>
   <sheetViews>
-    <sheetView topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="A87" sqref="A87"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3278,8 +3277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB032CAA-BD0C-4DC9-A38A-BDE275360C9C}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>